<commit_message>
update int to long
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/history/historyCompletedTestData.xlsx
+++ b/src/test/java/testCases/history/historyCompletedTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/otp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/history/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CB71B-339A-0640-8948-D1CA482813D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1C84AA-D4D1-B740-8A9B-3D01739537C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,9 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>id</t>
+    <t>page</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -456,11 +459,15 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+      <c r="A3" s="5">
+        <v>9999</v>
+      </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
     </row>

</xml_diff>

<commit_message>
update excel test data
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/history/historyCompletedTestData.xlsx
+++ b/src/test/java/testCases/history/historyCompletedTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/history/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1C84AA-D4D1-B740-8A9B-3D01739537C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EE0939-B0EF-1E41-A7F4-AAA06CD8530C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
@@ -33,12 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>page</t>
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,15 +455,15 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>9999</v>
+      <c r="A3" s="6">
+        <v>-1</v>
       </c>
       <c r="B3" s="2"/>
     </row>
@@ -472,10 +475,14 @@
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6">
+        <v>9999</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
@@ -497,5 +504,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>